<commit_message>
fixed values (from 0.01 to 10 to express percentage
</commit_message>
<xml_diff>
--- a/Simple_XLS_Importer/data/OKI-GODI/2016-OKI-GODI.xlsx
+++ b/Simple_XLS_Importer/data/OKI-GODI/2016-OKI-GODI.xlsx
@@ -5,7 +5,7 @@
   <workbookPr hidePivotFieldList="1" autoCompressPictures="0" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\carlos\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\carlos\Documents\projects\landbook-importers\Simple_XLS_Importer\data\OKI-GODI\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -15,7 +15,7 @@
     <sheet name="data" sheetId="3" r:id="rId1"/>
     <sheet name="metadata" sheetId="4" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="162913" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -2838,10 +2838,10 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2262">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8" hidden="1"/>
@@ -5409,8 +5409,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I447"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A159" zoomScaleNormal="100" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="A161" sqref="A161:XFD161"/>
+    <sheetView tabSelected="1" topLeftCell="A33" zoomScaleNormal="100" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="D95" sqref="D95:D187"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.44140625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -5454,7 +5454,7 @@
       <c r="D2">
         <v>1</v>
       </c>
-      <c r="E2" s="16" t="s">
+      <c r="E2" s="15" t="s">
         <v>40</v>
       </c>
       <c r="F2" s="1"/>
@@ -5475,7 +5475,7 @@
       <c r="D3">
         <v>2</v>
       </c>
-      <c r="E3" s="16" t="s">
+      <c r="E3" s="15" t="s">
         <v>42</v>
       </c>
     </row>
@@ -5492,7 +5492,7 @@
       <c r="D4">
         <v>3</v>
       </c>
-      <c r="E4" s="16" t="s">
+      <c r="E4" s="15" t="s">
         <v>44</v>
       </c>
     </row>
@@ -5509,7 +5509,7 @@
       <c r="D5">
         <v>3</v>
       </c>
-      <c r="E5" s="16" t="s">
+      <c r="E5" s="15" t="s">
         <v>46</v>
       </c>
     </row>
@@ -5526,7 +5526,7 @@
       <c r="D6">
         <v>3</v>
       </c>
-      <c r="E6" s="16" t="s">
+      <c r="E6" s="15" t="s">
         <v>48</v>
       </c>
     </row>
@@ -5543,7 +5543,7 @@
       <c r="D7">
         <v>6</v>
       </c>
-      <c r="E7" s="16" t="s">
+      <c r="E7" s="15" t="s">
         <v>49</v>
       </c>
     </row>
@@ -5560,7 +5560,7 @@
       <c r="D8">
         <v>6</v>
       </c>
-      <c r="E8" s="16" t="s">
+      <c r="E8" s="15" t="s">
         <v>51</v>
       </c>
     </row>
@@ -5577,7 +5577,7 @@
       <c r="D9">
         <v>6</v>
       </c>
-      <c r="E9" s="16" t="s">
+      <c r="E9" s="15" t="s">
         <v>51</v>
       </c>
     </row>
@@ -5594,7 +5594,7 @@
       <c r="D10">
         <v>6</v>
       </c>
-      <c r="E10" s="16" t="s">
+      <c r="E10" s="15" t="s">
         <v>51</v>
       </c>
     </row>
@@ -5611,7 +5611,7 @@
       <c r="D11">
         <v>10</v>
       </c>
-      <c r="E11" s="16" t="s">
+      <c r="E11" s="15" t="s">
         <v>55</v>
       </c>
     </row>
@@ -5628,7 +5628,7 @@
       <c r="D12">
         <v>10</v>
       </c>
-      <c r="E12" s="16" t="s">
+      <c r="E12" s="15" t="s">
         <v>55</v>
       </c>
     </row>
@@ -5645,7 +5645,7 @@
       <c r="D13">
         <v>12</v>
       </c>
-      <c r="E13" s="16" t="s">
+      <c r="E13" s="15" t="s">
         <v>58</v>
       </c>
     </row>
@@ -5662,7 +5662,7 @@
       <c r="D14">
         <v>12</v>
       </c>
-      <c r="E14" s="16" t="s">
+      <c r="E14" s="15" t="s">
         <v>58</v>
       </c>
     </row>
@@ -5679,7 +5679,7 @@
       <c r="D15">
         <v>12</v>
       </c>
-      <c r="E15" s="16" t="s">
+      <c r="E15" s="15" t="s">
         <v>58</v>
       </c>
     </row>
@@ -5696,7 +5696,7 @@
       <c r="D16">
         <v>15</v>
       </c>
-      <c r="E16" s="16" t="s">
+      <c r="E16" s="15" t="s">
         <v>62</v>
       </c>
     </row>
@@ -5713,7 +5713,7 @@
       <c r="D17">
         <v>15</v>
       </c>
-      <c r="E17" s="16" t="s">
+      <c r="E17" s="15" t="s">
         <v>62</v>
       </c>
     </row>
@@ -5730,7 +5730,7 @@
       <c r="D18">
         <v>15</v>
       </c>
-      <c r="E18" s="16" t="s">
+      <c r="E18" s="15" t="s">
         <v>62</v>
       </c>
     </row>
@@ -5747,7 +5747,7 @@
       <c r="D19">
         <v>18</v>
       </c>
-      <c r="E19" s="16" t="s">
+      <c r="E19" s="15" t="s">
         <v>65</v>
       </c>
     </row>
@@ -5764,7 +5764,7 @@
       <c r="D20">
         <v>18</v>
       </c>
-      <c r="E20" s="16" t="s">
+      <c r="E20" s="15" t="s">
         <v>65</v>
       </c>
     </row>
@@ -5781,7 +5781,7 @@
       <c r="D21">
         <v>18</v>
       </c>
-      <c r="E21" s="16" t="s">
+      <c r="E21" s="15" t="s">
         <v>65</v>
       </c>
     </row>
@@ -5798,7 +5798,7 @@
       <c r="D22">
         <v>18</v>
       </c>
-      <c r="E22" s="16" t="s">
+      <c r="E22" s="15" t="s">
         <v>65</v>
       </c>
     </row>
@@ -5815,7 +5815,7 @@
       <c r="D23">
         <v>18</v>
       </c>
-      <c r="E23" s="16" t="s">
+      <c r="E23" s="15" t="s">
         <v>65</v>
       </c>
     </row>
@@ -5832,7 +5832,7 @@
       <c r="D24">
         <v>18</v>
       </c>
-      <c r="E24" s="16" t="s">
+      <c r="E24" s="15" t="s">
         <v>65</v>
       </c>
     </row>
@@ -5849,7 +5849,7 @@
       <c r="D25">
         <v>18</v>
       </c>
-      <c r="E25" s="16" t="s">
+      <c r="E25" s="15" t="s">
         <v>65</v>
       </c>
     </row>
@@ -5866,7 +5866,7 @@
       <c r="D26">
         <v>18</v>
       </c>
-      <c r="E26" s="16" t="s">
+      <c r="E26" s="15" t="s">
         <v>65</v>
       </c>
     </row>
@@ -5883,7 +5883,7 @@
       <c r="D27">
         <v>18</v>
       </c>
-      <c r="E27" s="16" t="s">
+      <c r="E27" s="15" t="s">
         <v>65</v>
       </c>
     </row>
@@ -5900,7 +5900,7 @@
       <c r="D28">
         <v>18</v>
       </c>
-      <c r="E28" s="16" t="s">
+      <c r="E28" s="15" t="s">
         <v>65</v>
       </c>
     </row>
@@ -5917,7 +5917,7 @@
       <c r="D29">
         <v>18</v>
       </c>
-      <c r="E29" s="16" t="s">
+      <c r="E29" s="15" t="s">
         <v>65</v>
       </c>
     </row>
@@ -5934,7 +5934,7 @@
       <c r="D30">
         <v>18</v>
       </c>
-      <c r="E30" s="16" t="s">
+      <c r="E30" s="15" t="s">
         <v>65</v>
       </c>
     </row>
@@ -5951,7 +5951,7 @@
       <c r="D31">
         <v>18</v>
       </c>
-      <c r="E31" s="16" t="s">
+      <c r="E31" s="15" t="s">
         <v>65</v>
       </c>
     </row>
@@ -5968,7 +5968,7 @@
       <c r="D32">
         <v>18</v>
       </c>
-      <c r="E32" s="16" t="s">
+      <c r="E32" s="15" t="s">
         <v>65</v>
       </c>
     </row>
@@ -5985,7 +5985,7 @@
       <c r="D33">
         <v>18</v>
       </c>
-      <c r="E33" s="16" t="s">
+      <c r="E33" s="15" t="s">
         <v>65</v>
       </c>
     </row>
@@ -6002,7 +6002,7 @@
       <c r="D34">
         <v>18</v>
       </c>
-      <c r="E34" s="16" t="s">
+      <c r="E34" s="15" t="s">
         <v>65</v>
       </c>
     </row>
@@ -6019,7 +6019,7 @@
       <c r="D35">
         <v>18</v>
       </c>
-      <c r="E35" s="16" t="s">
+      <c r="E35" s="15" t="s">
         <v>65</v>
       </c>
     </row>
@@ -6036,7 +6036,7 @@
       <c r="D36">
         <v>18</v>
       </c>
-      <c r="E36" s="16" t="s">
+      <c r="E36" s="15" t="s">
         <v>65</v>
       </c>
     </row>
@@ -6053,7 +6053,7 @@
       <c r="D37">
         <v>18</v>
       </c>
-      <c r="E37" s="16" t="s">
+      <c r="E37" s="15" t="s">
         <v>65</v>
       </c>
     </row>
@@ -6070,7 +6070,7 @@
       <c r="D38">
         <v>18</v>
       </c>
-      <c r="E38" s="16" t="s">
+      <c r="E38" s="15" t="s">
         <v>65</v>
       </c>
     </row>
@@ -6087,7 +6087,7 @@
       <c r="D39">
         <v>18</v>
       </c>
-      <c r="E39" s="16" t="s">
+      <c r="E39" s="15" t="s">
         <v>65</v>
       </c>
     </row>
@@ -6104,7 +6104,7 @@
       <c r="D40">
         <v>18</v>
       </c>
-      <c r="E40" s="16" t="s">
+      <c r="E40" s="15" t="s">
         <v>65</v>
       </c>
     </row>
@@ -6121,7 +6121,7 @@
       <c r="D41">
         <v>18</v>
       </c>
-      <c r="E41" s="16" t="s">
+      <c r="E41" s="15" t="s">
         <v>65</v>
       </c>
     </row>
@@ -6138,7 +6138,7 @@
       <c r="D42">
         <v>18</v>
       </c>
-      <c r="E42" s="16" t="s">
+      <c r="E42" s="15" t="s">
         <v>65</v>
       </c>
     </row>
@@ -6155,7 +6155,7 @@
       <c r="D43">
         <v>18</v>
       </c>
-      <c r="E43" s="16" t="s">
+      <c r="E43" s="15" t="s">
         <v>65</v>
       </c>
     </row>
@@ -6172,7 +6172,7 @@
       <c r="D44">
         <v>18</v>
       </c>
-      <c r="E44" s="16" t="s">
+      <c r="E44" s="15" t="s">
         <v>65</v>
       </c>
     </row>
@@ -6189,7 +6189,7 @@
       <c r="D45">
         <v>18</v>
       </c>
-      <c r="E45" s="16" t="s">
+      <c r="E45" s="15" t="s">
         <v>65</v>
       </c>
     </row>
@@ -6206,7 +6206,7 @@
       <c r="D46">
         <v>18</v>
       </c>
-      <c r="E46" s="16" t="s">
+      <c r="E46" s="15" t="s">
         <v>65</v>
       </c>
     </row>
@@ -6223,7 +6223,7 @@
       <c r="D47">
         <v>18</v>
       </c>
-      <c r="E47" s="16" t="s">
+      <c r="E47" s="15" t="s">
         <v>65</v>
       </c>
     </row>
@@ -6240,7 +6240,7 @@
       <c r="D48">
         <v>18</v>
       </c>
-      <c r="E48" s="16" t="s">
+      <c r="E48" s="15" t="s">
         <v>65</v>
       </c>
     </row>
@@ -6257,7 +6257,7 @@
       <c r="D49">
         <v>18</v>
       </c>
-      <c r="E49" s="16" t="s">
+      <c r="E49" s="15" t="s">
         <v>65</v>
       </c>
     </row>
@@ -6274,7 +6274,7 @@
       <c r="D50">
         <v>18</v>
       </c>
-      <c r="E50" s="16" t="s">
+      <c r="E50" s="15" t="s">
         <v>65</v>
       </c>
     </row>
@@ -6291,7 +6291,7 @@
       <c r="D51">
         <v>18</v>
       </c>
-      <c r="E51" s="16" t="s">
+      <c r="E51" s="15" t="s">
         <v>65</v>
       </c>
     </row>
@@ -6308,7 +6308,7 @@
       <c r="D52">
         <v>18</v>
       </c>
-      <c r="E52" s="16" t="s">
+      <c r="E52" s="15" t="s">
         <v>65</v>
       </c>
     </row>
@@ -6325,7 +6325,7 @@
       <c r="D53">
         <v>18</v>
       </c>
-      <c r="E53" s="16" t="s">
+      <c r="E53" s="15" t="s">
         <v>65</v>
       </c>
     </row>
@@ -6342,7 +6342,7 @@
       <c r="D54">
         <v>18</v>
       </c>
-      <c r="E54" s="16" t="s">
+      <c r="E54" s="15" t="s">
         <v>65</v>
       </c>
     </row>
@@ -6359,7 +6359,7 @@
       <c r="D55">
         <v>18</v>
       </c>
-      <c r="E55" s="16" t="s">
+      <c r="E55" s="15" t="s">
         <v>65</v>
       </c>
     </row>
@@ -6376,7 +6376,7 @@
       <c r="D56">
         <v>18</v>
       </c>
-      <c r="E56" s="16" t="s">
+      <c r="E56" s="15" t="s">
         <v>65</v>
       </c>
     </row>
@@ -6393,7 +6393,7 @@
       <c r="D57">
         <v>18</v>
       </c>
-      <c r="E57" s="16" t="s">
+      <c r="E57" s="15" t="s">
         <v>65</v>
       </c>
     </row>
@@ -6410,7 +6410,7 @@
       <c r="D58">
         <v>18</v>
       </c>
-      <c r="E58" s="16" t="s">
+      <c r="E58" s="15" t="s">
         <v>65</v>
       </c>
     </row>
@@ -6427,7 +6427,7 @@
       <c r="D59">
         <v>18</v>
       </c>
-      <c r="E59" s="16" t="s">
+      <c r="E59" s="15" t="s">
         <v>65</v>
       </c>
     </row>
@@ -6444,7 +6444,7 @@
       <c r="D60">
         <v>18</v>
       </c>
-      <c r="E60" s="16" t="s">
+      <c r="E60" s="15" t="s">
         <v>65</v>
       </c>
     </row>
@@ -6461,7 +6461,7 @@
       <c r="D61">
         <v>18</v>
       </c>
-      <c r="E61" s="16" t="s">
+      <c r="E61" s="15" t="s">
         <v>65</v>
       </c>
     </row>
@@ -6478,7 +6478,7 @@
       <c r="D62">
         <v>18</v>
       </c>
-      <c r="E62" s="16" t="s">
+      <c r="E62" s="15" t="s">
         <v>65</v>
       </c>
     </row>
@@ -6495,7 +6495,7 @@
       <c r="D63">
         <v>18</v>
       </c>
-      <c r="E63" s="16" t="s">
+      <c r="E63" s="15" t="s">
         <v>65</v>
       </c>
     </row>
@@ -6512,7 +6512,7 @@
       <c r="D64">
         <v>18</v>
       </c>
-      <c r="E64" s="16" t="s">
+      <c r="E64" s="15" t="s">
         <v>65</v>
       </c>
     </row>
@@ -6529,7 +6529,7 @@
       <c r="D65">
         <v>18</v>
       </c>
-      <c r="E65" s="16" t="s">
+      <c r="E65" s="15" t="s">
         <v>65</v>
       </c>
     </row>
@@ -6546,7 +6546,7 @@
       <c r="D66">
         <v>18</v>
       </c>
-      <c r="E66" s="16" t="s">
+      <c r="E66" s="15" t="s">
         <v>65</v>
       </c>
     </row>
@@ -6563,7 +6563,7 @@
       <c r="D67">
         <v>18</v>
       </c>
-      <c r="E67" s="16" t="s">
+      <c r="E67" s="15" t="s">
         <v>65</v>
       </c>
     </row>
@@ -6580,7 +6580,7 @@
       <c r="D68">
         <v>18</v>
       </c>
-      <c r="E68" s="16" t="s">
+      <c r="E68" s="15" t="s">
         <v>65</v>
       </c>
     </row>
@@ -6597,7 +6597,7 @@
       <c r="D69">
         <v>18</v>
       </c>
-      <c r="E69" s="16" t="s">
+      <c r="E69" s="15" t="s">
         <v>65</v>
       </c>
     </row>
@@ -6614,7 +6614,7 @@
       <c r="D70">
         <v>18</v>
       </c>
-      <c r="E70" s="16" t="s">
+      <c r="E70" s="15" t="s">
         <v>65</v>
       </c>
     </row>
@@ -6631,7 +6631,7 @@
       <c r="D71">
         <v>18</v>
       </c>
-      <c r="E71" s="16" t="s">
+      <c r="E71" s="15" t="s">
         <v>65</v>
       </c>
     </row>
@@ -6648,7 +6648,7 @@
       <c r="D72">
         <v>18</v>
       </c>
-      <c r="E72" s="16" t="s">
+      <c r="E72" s="15" t="s">
         <v>65</v>
       </c>
     </row>
@@ -6665,7 +6665,7 @@
       <c r="D73">
         <v>18</v>
       </c>
-      <c r="E73" s="16" t="s">
+      <c r="E73" s="15" t="s">
         <v>65</v>
       </c>
     </row>
@@ -6682,7 +6682,7 @@
       <c r="D74">
         <v>18</v>
       </c>
-      <c r="E74" s="16" t="s">
+      <c r="E74" s="15" t="s">
         <v>65</v>
       </c>
     </row>
@@ -6699,7 +6699,7 @@
       <c r="D75">
         <v>18</v>
       </c>
-      <c r="E75" s="16" t="s">
+      <c r="E75" s="15" t="s">
         <v>65</v>
       </c>
     </row>
@@ -6716,7 +6716,7 @@
       <c r="D76">
         <v>18</v>
       </c>
-      <c r="E76" s="16" t="s">
+      <c r="E76" s="15" t="s">
         <v>65</v>
       </c>
     </row>
@@ -6733,7 +6733,7 @@
       <c r="D77">
         <v>18</v>
       </c>
-      <c r="E77" s="16" t="s">
+      <c r="E77" s="15" t="s">
         <v>65</v>
       </c>
     </row>
@@ -6750,7 +6750,7 @@
       <c r="D78">
         <v>18</v>
       </c>
-      <c r="E78" s="16" t="s">
+      <c r="E78" s="15" t="s">
         <v>65</v>
       </c>
     </row>
@@ -6767,7 +6767,7 @@
       <c r="D79">
         <v>18</v>
       </c>
-      <c r="E79" s="16" t="s">
+      <c r="E79" s="15" t="s">
         <v>65</v>
       </c>
     </row>
@@ -6784,7 +6784,7 @@
       <c r="D80">
         <v>18</v>
       </c>
-      <c r="E80" s="16" t="s">
+      <c r="E80" s="15" t="s">
         <v>65</v>
       </c>
     </row>
@@ -6801,7 +6801,7 @@
       <c r="D81">
         <v>18</v>
       </c>
-      <c r="E81" s="16" t="s">
+      <c r="E81" s="15" t="s">
         <v>65</v>
       </c>
     </row>
@@ -6818,7 +6818,7 @@
       <c r="D82">
         <v>18</v>
       </c>
-      <c r="E82" s="16" t="s">
+      <c r="E82" s="15" t="s">
         <v>65</v>
       </c>
     </row>
@@ -6835,7 +6835,7 @@
       <c r="D83">
         <v>18</v>
       </c>
-      <c r="E83" s="16" t="s">
+      <c r="E83" s="15" t="s">
         <v>65</v>
       </c>
     </row>
@@ -6852,7 +6852,7 @@
       <c r="D84">
         <v>18</v>
       </c>
-      <c r="E84" s="16" t="s">
+      <c r="E84" s="15" t="s">
         <v>65</v>
       </c>
     </row>
@@ -6869,7 +6869,7 @@
       <c r="D85">
         <v>18</v>
       </c>
-      <c r="E85" s="16" t="s">
+      <c r="E85" s="15" t="s">
         <v>65</v>
       </c>
     </row>
@@ -6886,7 +6886,7 @@
       <c r="D86">
         <v>18</v>
       </c>
-      <c r="E86" s="16" t="s">
+      <c r="E86" s="15" t="s">
         <v>65</v>
       </c>
     </row>
@@ -6903,7 +6903,7 @@
       <c r="D87">
         <v>18</v>
       </c>
-      <c r="E87" s="16" t="s">
+      <c r="E87" s="15" t="s">
         <v>65</v>
       </c>
     </row>
@@ -6920,7 +6920,7 @@
       <c r="D88">
         <v>18</v>
       </c>
-      <c r="E88" s="16" t="s">
+      <c r="E88" s="15" t="s">
         <v>65</v>
       </c>
     </row>
@@ -6937,7 +6937,7 @@
       <c r="D89">
         <v>18</v>
       </c>
-      <c r="E89" s="16" t="s">
+      <c r="E89" s="15" t="s">
         <v>65</v>
       </c>
     </row>
@@ -6954,7 +6954,7 @@
       <c r="D90">
         <v>18</v>
       </c>
-      <c r="E90" s="16" t="s">
+      <c r="E90" s="15" t="s">
         <v>65</v>
       </c>
     </row>
@@ -6971,7 +6971,7 @@
       <c r="D91">
         <v>18</v>
       </c>
-      <c r="E91" s="16" t="s">
+      <c r="E91" s="15" t="s">
         <v>65</v>
       </c>
     </row>
@@ -6988,7 +6988,7 @@
       <c r="D92">
         <v>18</v>
       </c>
-      <c r="E92" s="16" t="s">
+      <c r="E92" s="15" t="s">
         <v>65</v>
       </c>
     </row>
@@ -7005,7 +7005,7 @@
       <c r="D93">
         <v>18</v>
       </c>
-      <c r="E93" s="16" t="s">
+      <c r="E93" s="15" t="s">
         <v>65</v>
       </c>
     </row>
@@ -7022,7 +7022,7 @@
       <c r="D94">
         <v>18</v>
       </c>
-      <c r="E94" s="16" t="s">
+      <c r="E94" s="15" t="s">
         <v>65</v>
       </c>
     </row>
@@ -7036,10 +7036,10 @@
       <c r="C95">
         <v>2016</v>
       </c>
-      <c r="D95" s="15">
-        <v>1</v>
-      </c>
-      <c r="E95" s="16" t="s">
+      <c r="D95" s="16">
+        <v>100</v>
+      </c>
+      <c r="E95" s="15" t="s">
         <v>40</v>
       </c>
     </row>
@@ -7053,10 +7053,10 @@
       <c r="C96">
         <v>2016</v>
       </c>
-      <c r="D96" s="15">
-        <v>0.85</v>
-      </c>
-      <c r="E96" s="16" t="s">
+      <c r="D96" s="16">
+        <v>85</v>
+      </c>
+      <c r="E96" s="15" t="s">
         <v>42</v>
       </c>
     </row>
@@ -7070,10 +7070,10 @@
       <c r="C97">
         <v>2016</v>
       </c>
-      <c r="D97" s="15">
-        <v>0.65</v>
-      </c>
-      <c r="E97" s="16" t="s">
+      <c r="D97" s="16">
+        <v>65</v>
+      </c>
+      <c r="E97" s="15" t="s">
         <v>44</v>
       </c>
     </row>
@@ -7087,10 +7087,10 @@
       <c r="C98">
         <v>2016</v>
       </c>
-      <c r="D98" s="15">
-        <v>0.65</v>
-      </c>
-      <c r="E98" s="16" t="s">
+      <c r="D98" s="16">
+        <v>65</v>
+      </c>
+      <c r="E98" s="15" t="s">
         <v>46</v>
       </c>
     </row>
@@ -7104,10 +7104,10 @@
       <c r="C99">
         <v>2016</v>
       </c>
-      <c r="D99" s="15">
-        <v>0.65</v>
-      </c>
-      <c r="E99" s="16" t="s">
+      <c r="D99" s="16">
+        <v>65</v>
+      </c>
+      <c r="E99" s="15" t="s">
         <v>48</v>
       </c>
     </row>
@@ -7121,10 +7121,10 @@
       <c r="C100">
         <v>2016</v>
       </c>
-      <c r="D100" s="15">
-        <v>0.45</v>
-      </c>
-      <c r="E100" s="16" t="s">
+      <c r="D100" s="16">
+        <v>45</v>
+      </c>
+      <c r="E100" s="15" t="s">
         <v>49</v>
       </c>
     </row>
@@ -7138,10 +7138,10 @@
       <c r="C101">
         <v>2016</v>
       </c>
-      <c r="D101" s="15">
-        <v>0.45</v>
-      </c>
-      <c r="E101" s="16" t="s">
+      <c r="D101" s="16">
+        <v>45</v>
+      </c>
+      <c r="E101" s="15" t="s">
         <v>51</v>
       </c>
     </row>
@@ -7155,10 +7155,10 @@
       <c r="C102">
         <v>2016</v>
       </c>
-      <c r="D102" s="15">
-        <v>0.45</v>
-      </c>
-      <c r="E102" s="16" t="s">
+      <c r="D102" s="16">
+        <v>45</v>
+      </c>
+      <c r="E102" s="15" t="s">
         <v>51</v>
       </c>
     </row>
@@ -7172,10 +7172,10 @@
       <c r="C103">
         <v>2016</v>
       </c>
-      <c r="D103" s="15">
-        <v>0.45</v>
-      </c>
-      <c r="E103" s="16" t="s">
+      <c r="D103" s="16">
+        <v>45</v>
+      </c>
+      <c r="E103" s="15" t="s">
         <v>51</v>
       </c>
     </row>
@@ -7189,10 +7189,10 @@
       <c r="C104">
         <v>2016</v>
       </c>
-      <c r="D104" s="15">
-        <v>0.35</v>
-      </c>
-      <c r="E104" s="16" t="s">
+      <c r="D104" s="16">
+        <v>35</v>
+      </c>
+      <c r="E104" s="15" t="s">
         <v>55</v>
       </c>
     </row>
@@ -7206,10 +7206,10 @@
       <c r="C105">
         <v>2016</v>
       </c>
-      <c r="D105" s="15">
-        <v>0.35</v>
-      </c>
-      <c r="E105" s="16" t="s">
+      <c r="D105" s="16">
+        <v>35</v>
+      </c>
+      <c r="E105" s="15" t="s">
         <v>55</v>
       </c>
     </row>
@@ -7223,10 +7223,10 @@
       <c r="C106">
         <v>2016</v>
       </c>
-      <c r="D106" s="15">
-        <v>0.3</v>
-      </c>
-      <c r="E106" s="16" t="s">
+      <c r="D106" s="16">
+        <v>30</v>
+      </c>
+      <c r="E106" s="15" t="s">
         <v>58</v>
       </c>
     </row>
@@ -7240,10 +7240,10 @@
       <c r="C107">
         <v>2016</v>
       </c>
-      <c r="D107" s="15">
-        <v>0.3</v>
-      </c>
-      <c r="E107" s="16" t="s">
+      <c r="D107" s="16">
+        <v>30</v>
+      </c>
+      <c r="E107" s="15" t="s">
         <v>58</v>
       </c>
     </row>
@@ -7257,10 +7257,10 @@
       <c r="C108">
         <v>2016</v>
       </c>
-      <c r="D108" s="15">
-        <v>0.3</v>
-      </c>
-      <c r="E108" s="16" t="s">
+      <c r="D108" s="16">
+        <v>30</v>
+      </c>
+      <c r="E108" s="15" t="s">
         <v>58</v>
       </c>
     </row>
@@ -7274,10 +7274,10 @@
       <c r="C109">
         <v>2016</v>
       </c>
-      <c r="D109" s="15">
-        <v>0.15</v>
-      </c>
-      <c r="E109" s="16" t="s">
+      <c r="D109" s="16">
+        <v>15</v>
+      </c>
+      <c r="E109" s="15" t="s">
         <v>62</v>
       </c>
     </row>
@@ -7291,10 +7291,10 @@
       <c r="C110">
         <v>2016</v>
       </c>
-      <c r="D110" s="15">
-        <v>0.15</v>
-      </c>
-      <c r="E110" s="16" t="s">
+      <c r="D110" s="16">
+        <v>15</v>
+      </c>
+      <c r="E110" s="15" t="s">
         <v>62</v>
       </c>
     </row>
@@ -7308,10 +7308,10 @@
       <c r="C111">
         <v>2016</v>
       </c>
-      <c r="D111" s="15">
-        <v>0.15</v>
-      </c>
-      <c r="E111" s="16" t="s">
+      <c r="D111" s="16">
+        <v>15</v>
+      </c>
+      <c r="E111" s="15" t="s">
         <v>62</v>
       </c>
     </row>
@@ -7325,10 +7325,10 @@
       <c r="C112">
         <v>2016</v>
       </c>
-      <c r="D112" s="15">
+      <c r="D112" s="16">
         <v>0</v>
       </c>
-      <c r="E112" s="16" t="s">
+      <c r="E112" s="15" t="s">
         <v>65</v>
       </c>
     </row>
@@ -7342,10 +7342,10 @@
       <c r="C113">
         <v>2016</v>
       </c>
-      <c r="D113" s="15">
+      <c r="D113" s="16">
         <v>0</v>
       </c>
-      <c r="E113" s="16" t="s">
+      <c r="E113" s="15" t="s">
         <v>65</v>
       </c>
     </row>
@@ -7359,10 +7359,10 @@
       <c r="C114">
         <v>2016</v>
       </c>
-      <c r="D114" s="15">
+      <c r="D114" s="16">
         <v>0</v>
       </c>
-      <c r="E114" s="16" t="s">
+      <c r="E114" s="15" t="s">
         <v>65</v>
       </c>
     </row>
@@ -7376,10 +7376,10 @@
       <c r="C115">
         <v>2016</v>
       </c>
-      <c r="D115" s="15">
+      <c r="D115" s="16">
         <v>0</v>
       </c>
-      <c r="E115" s="16" t="s">
+      <c r="E115" s="15" t="s">
         <v>65</v>
       </c>
     </row>
@@ -7393,10 +7393,10 @@
       <c r="C116">
         <v>2016</v>
       </c>
-      <c r="D116" s="15">
+      <c r="D116" s="16">
         <v>0</v>
       </c>
-      <c r="E116" s="16" t="s">
+      <c r="E116" s="15" t="s">
         <v>65</v>
       </c>
     </row>
@@ -7410,10 +7410,10 @@
       <c r="C117">
         <v>2016</v>
       </c>
-      <c r="D117" s="15">
+      <c r="D117" s="16">
         <v>0</v>
       </c>
-      <c r="E117" s="16" t="s">
+      <c r="E117" s="15" t="s">
         <v>65</v>
       </c>
     </row>
@@ -7427,10 +7427,10 @@
       <c r="C118">
         <v>2016</v>
       </c>
-      <c r="D118" s="15">
+      <c r="D118" s="16">
         <v>0</v>
       </c>
-      <c r="E118" s="16" t="s">
+      <c r="E118" s="15" t="s">
         <v>65</v>
       </c>
     </row>
@@ -7444,10 +7444,10 @@
       <c r="C119">
         <v>2016</v>
       </c>
-      <c r="D119" s="15">
+      <c r="D119" s="16">
         <v>0</v>
       </c>
-      <c r="E119" s="16" t="s">
+      <c r="E119" s="15" t="s">
         <v>65</v>
       </c>
     </row>
@@ -7461,10 +7461,10 @@
       <c r="C120">
         <v>2016</v>
       </c>
-      <c r="D120" s="15">
+      <c r="D120" s="16">
         <v>0</v>
       </c>
-      <c r="E120" s="16" t="s">
+      <c r="E120" s="15" t="s">
         <v>65</v>
       </c>
     </row>
@@ -7478,10 +7478,10 @@
       <c r="C121">
         <v>2016</v>
       </c>
-      <c r="D121" s="15">
+      <c r="D121" s="16">
         <v>0</v>
       </c>
-      <c r="E121" s="16" t="s">
+      <c r="E121" s="15" t="s">
         <v>65</v>
       </c>
     </row>
@@ -7495,10 +7495,10 @@
       <c r="C122">
         <v>2016</v>
       </c>
-      <c r="D122" s="15">
+      <c r="D122" s="16">
         <v>0</v>
       </c>
-      <c r="E122" s="16" t="s">
+      <c r="E122" s="15" t="s">
         <v>65</v>
       </c>
     </row>
@@ -7512,10 +7512,10 @@
       <c r="C123">
         <v>2016</v>
       </c>
-      <c r="D123" s="15">
+      <c r="D123" s="16">
         <v>0</v>
       </c>
-      <c r="E123" s="16" t="s">
+      <c r="E123" s="15" t="s">
         <v>65</v>
       </c>
     </row>
@@ -7529,10 +7529,10 @@
       <c r="C124">
         <v>2016</v>
       </c>
-      <c r="D124" s="15">
+      <c r="D124" s="16">
         <v>0</v>
       </c>
-      <c r="E124" s="16" t="s">
+      <c r="E124" s="15" t="s">
         <v>65</v>
       </c>
     </row>
@@ -7546,10 +7546,10 @@
       <c r="C125">
         <v>2016</v>
       </c>
-      <c r="D125" s="15">
+      <c r="D125" s="16">
         <v>0</v>
       </c>
-      <c r="E125" s="16" t="s">
+      <c r="E125" s="15" t="s">
         <v>65</v>
       </c>
     </row>
@@ -7563,10 +7563,10 @@
       <c r="C126">
         <v>2016</v>
       </c>
-      <c r="D126" s="15">
+      <c r="D126" s="16">
         <v>0</v>
       </c>
-      <c r="E126" s="16" t="s">
+      <c r="E126" s="15" t="s">
         <v>65</v>
       </c>
     </row>
@@ -7580,10 +7580,10 @@
       <c r="C127">
         <v>2016</v>
       </c>
-      <c r="D127" s="15">
+      <c r="D127" s="16">
         <v>0</v>
       </c>
-      <c r="E127" s="16" t="s">
+      <c r="E127" s="15" t="s">
         <v>65</v>
       </c>
     </row>
@@ -7597,10 +7597,10 @@
       <c r="C128">
         <v>2016</v>
       </c>
-      <c r="D128" s="15">
+      <c r="D128" s="16">
         <v>0</v>
       </c>
-      <c r="E128" s="16" t="s">
+      <c r="E128" s="15" t="s">
         <v>65</v>
       </c>
     </row>
@@ -7614,10 +7614,10 @@
       <c r="C129">
         <v>2016</v>
       </c>
-      <c r="D129" s="15">
+      <c r="D129" s="16">
         <v>0</v>
       </c>
-      <c r="E129" s="16" t="s">
+      <c r="E129" s="15" t="s">
         <v>65</v>
       </c>
     </row>
@@ -7631,10 +7631,10 @@
       <c r="C130">
         <v>2016</v>
       </c>
-      <c r="D130" s="15">
+      <c r="D130" s="16">
         <v>0</v>
       </c>
-      <c r="E130" s="16" t="s">
+      <c r="E130" s="15" t="s">
         <v>65</v>
       </c>
     </row>
@@ -7648,10 +7648,10 @@
       <c r="C131">
         <v>2016</v>
       </c>
-      <c r="D131" s="15">
+      <c r="D131" s="16">
         <v>0</v>
       </c>
-      <c r="E131" s="16" t="s">
+      <c r="E131" s="15" t="s">
         <v>65</v>
       </c>
     </row>
@@ -7665,10 +7665,10 @@
       <c r="C132">
         <v>2016</v>
       </c>
-      <c r="D132" s="15">
+      <c r="D132" s="16">
         <v>0</v>
       </c>
-      <c r="E132" s="16" t="s">
+      <c r="E132" s="15" t="s">
         <v>65</v>
       </c>
     </row>
@@ -7682,10 +7682,10 @@
       <c r="C133">
         <v>2016</v>
       </c>
-      <c r="D133" s="15">
+      <c r="D133" s="16">
         <v>0</v>
       </c>
-      <c r="E133" s="16" t="s">
+      <c r="E133" s="15" t="s">
         <v>65</v>
       </c>
     </row>
@@ -7699,10 +7699,10 @@
       <c r="C134">
         <v>2016</v>
       </c>
-      <c r="D134" s="15">
+      <c r="D134" s="16">
         <v>0</v>
       </c>
-      <c r="E134" s="16" t="s">
+      <c r="E134" s="15" t="s">
         <v>65</v>
       </c>
     </row>
@@ -7716,10 +7716,10 @@
       <c r="C135">
         <v>2016</v>
       </c>
-      <c r="D135" s="15">
+      <c r="D135" s="16">
         <v>0</v>
       </c>
-      <c r="E135" s="16" t="s">
+      <c r="E135" s="15" t="s">
         <v>65</v>
       </c>
     </row>
@@ -7733,10 +7733,10 @@
       <c r="C136">
         <v>2016</v>
       </c>
-      <c r="D136" s="15">
+      <c r="D136" s="16">
         <v>0</v>
       </c>
-      <c r="E136" s="16" t="s">
+      <c r="E136" s="15" t="s">
         <v>65</v>
       </c>
     </row>
@@ -7750,10 +7750,10 @@
       <c r="C137">
         <v>2016</v>
       </c>
-      <c r="D137" s="15">
+      <c r="D137" s="16">
         <v>0</v>
       </c>
-      <c r="E137" s="16" t="s">
+      <c r="E137" s="15" t="s">
         <v>65</v>
       </c>
     </row>
@@ -7767,10 +7767,10 @@
       <c r="C138">
         <v>2016</v>
       </c>
-      <c r="D138" s="15">
+      <c r="D138" s="16">
         <v>0</v>
       </c>
-      <c r="E138" s="16" t="s">
+      <c r="E138" s="15" t="s">
         <v>65</v>
       </c>
     </row>
@@ -7784,10 +7784,10 @@
       <c r="C139">
         <v>2016</v>
       </c>
-      <c r="D139" s="15">
+      <c r="D139" s="16">
         <v>0</v>
       </c>
-      <c r="E139" s="16" t="s">
+      <c r="E139" s="15" t="s">
         <v>65</v>
       </c>
     </row>
@@ -7801,10 +7801,10 @@
       <c r="C140">
         <v>2016</v>
       </c>
-      <c r="D140" s="15">
+      <c r="D140" s="16">
         <v>0</v>
       </c>
-      <c r="E140" s="16" t="s">
+      <c r="E140" s="15" t="s">
         <v>65</v>
       </c>
     </row>
@@ -7818,10 +7818,10 @@
       <c r="C141">
         <v>2016</v>
       </c>
-      <c r="D141" s="15">
+      <c r="D141" s="16">
         <v>0</v>
       </c>
-      <c r="E141" s="16" t="s">
+      <c r="E141" s="15" t="s">
         <v>65</v>
       </c>
     </row>
@@ -7835,10 +7835,10 @@
       <c r="C142">
         <v>2016</v>
       </c>
-      <c r="D142" s="15">
+      <c r="D142" s="16">
         <v>0</v>
       </c>
-      <c r="E142" s="16" t="s">
+      <c r="E142" s="15" t="s">
         <v>65</v>
       </c>
     </row>
@@ -7852,10 +7852,10 @@
       <c r="C143">
         <v>2016</v>
       </c>
-      <c r="D143" s="15">
+      <c r="D143" s="16">
         <v>0</v>
       </c>
-      <c r="E143" s="16" t="s">
+      <c r="E143" s="15" t="s">
         <v>65</v>
       </c>
     </row>
@@ -7869,10 +7869,10 @@
       <c r="C144">
         <v>2016</v>
       </c>
-      <c r="D144" s="15">
+      <c r="D144" s="16">
         <v>0</v>
       </c>
-      <c r="E144" s="16" t="s">
+      <c r="E144" s="15" t="s">
         <v>65</v>
       </c>
     </row>
@@ -7886,10 +7886,10 @@
       <c r="C145">
         <v>2016</v>
       </c>
-      <c r="D145" s="15">
+      <c r="D145" s="16">
         <v>0</v>
       </c>
-      <c r="E145" s="16" t="s">
+      <c r="E145" s="15" t="s">
         <v>65</v>
       </c>
     </row>
@@ -7903,10 +7903,10 @@
       <c r="C146">
         <v>2016</v>
       </c>
-      <c r="D146" s="15">
+      <c r="D146" s="16">
         <v>0</v>
       </c>
-      <c r="E146" s="16" t="s">
+      <c r="E146" s="15" t="s">
         <v>65</v>
       </c>
     </row>
@@ -7920,10 +7920,10 @@
       <c r="C147">
         <v>2016</v>
       </c>
-      <c r="D147" s="15">
+      <c r="D147" s="16">
         <v>0</v>
       </c>
-      <c r="E147" s="16" t="s">
+      <c r="E147" s="15" t="s">
         <v>65</v>
       </c>
     </row>
@@ -7937,10 +7937,10 @@
       <c r="C148">
         <v>2016</v>
       </c>
-      <c r="D148" s="15">
+      <c r="D148" s="16">
         <v>0</v>
       </c>
-      <c r="E148" s="16" t="s">
+      <c r="E148" s="15" t="s">
         <v>65</v>
       </c>
     </row>
@@ -7954,10 +7954,10 @@
       <c r="C149">
         <v>2016</v>
       </c>
-      <c r="D149" s="15">
+      <c r="D149" s="16">
         <v>0</v>
       </c>
-      <c r="E149" s="16" t="s">
+      <c r="E149" s="15" t="s">
         <v>65</v>
       </c>
     </row>
@@ -7971,10 +7971,10 @@
       <c r="C150">
         <v>2016</v>
       </c>
-      <c r="D150" s="15">
+      <c r="D150" s="16">
         <v>0</v>
       </c>
-      <c r="E150" s="16" t="s">
+      <c r="E150" s="15" t="s">
         <v>65</v>
       </c>
     </row>
@@ -7988,10 +7988,10 @@
       <c r="C151">
         <v>2016</v>
       </c>
-      <c r="D151" s="15">
+      <c r="D151" s="16">
         <v>0</v>
       </c>
-      <c r="E151" s="16" t="s">
+      <c r="E151" s="15" t="s">
         <v>65</v>
       </c>
     </row>
@@ -8005,10 +8005,10 @@
       <c r="C152">
         <v>2016</v>
       </c>
-      <c r="D152" s="15">
+      <c r="D152" s="16">
         <v>0</v>
       </c>
-      <c r="E152" s="16" t="s">
+      <c r="E152" s="15" t="s">
         <v>65</v>
       </c>
     </row>
@@ -8022,10 +8022,10 @@
       <c r="C153">
         <v>2016</v>
       </c>
-      <c r="D153" s="15">
+      <c r="D153" s="16">
         <v>0</v>
       </c>
-      <c r="E153" s="16" t="s">
+      <c r="E153" s="15" t="s">
         <v>65</v>
       </c>
     </row>
@@ -8039,10 +8039,10 @@
       <c r="C154">
         <v>2016</v>
       </c>
-      <c r="D154" s="15">
+      <c r="D154" s="16">
         <v>0</v>
       </c>
-      <c r="E154" s="16" t="s">
+      <c r="E154" s="15" t="s">
         <v>65</v>
       </c>
     </row>
@@ -8056,10 +8056,10 @@
       <c r="C155">
         <v>2016</v>
       </c>
-      <c r="D155" s="15">
+      <c r="D155" s="16">
         <v>0</v>
       </c>
-      <c r="E155" s="16" t="s">
+      <c r="E155" s="15" t="s">
         <v>65</v>
       </c>
     </row>
@@ -8073,10 +8073,10 @@
       <c r="C156">
         <v>2016</v>
       </c>
-      <c r="D156" s="15">
+      <c r="D156" s="16">
         <v>0</v>
       </c>
-      <c r="E156" s="16" t="s">
+      <c r="E156" s="15" t="s">
         <v>65</v>
       </c>
     </row>
@@ -8090,10 +8090,10 @@
       <c r="C157">
         <v>2016</v>
       </c>
-      <c r="D157" s="15">
+      <c r="D157" s="16">
         <v>0</v>
       </c>
-      <c r="E157" s="16" t="s">
+      <c r="E157" s="15" t="s">
         <v>65</v>
       </c>
     </row>
@@ -8107,10 +8107,10 @@
       <c r="C158">
         <v>2016</v>
       </c>
-      <c r="D158" s="15">
+      <c r="D158" s="16">
         <v>0</v>
       </c>
-      <c r="E158" s="16" t="s">
+      <c r="E158" s="15" t="s">
         <v>65</v>
       </c>
     </row>
@@ -8124,10 +8124,10 @@
       <c r="C159">
         <v>2016</v>
       </c>
-      <c r="D159" s="15">
+      <c r="D159" s="16">
         <v>0</v>
       </c>
-      <c r="E159" s="16" t="s">
+      <c r="E159" s="15" t="s">
         <v>65</v>
       </c>
     </row>
@@ -8141,10 +8141,10 @@
       <c r="C160">
         <v>2016</v>
       </c>
-      <c r="D160" s="15">
+      <c r="D160" s="16">
         <v>0</v>
       </c>
-      <c r="E160" s="16" t="s">
+      <c r="E160" s="15" t="s">
         <v>65</v>
       </c>
     </row>
@@ -8158,10 +8158,10 @@
       <c r="C161">
         <v>2016</v>
       </c>
-      <c r="D161" s="15">
+      <c r="D161" s="16">
         <v>0</v>
       </c>
-      <c r="E161" s="16" t="s">
+      <c r="E161" s="15" t="s">
         <v>65</v>
       </c>
     </row>
@@ -8175,10 +8175,10 @@
       <c r="C162">
         <v>2016</v>
       </c>
-      <c r="D162" s="15">
+      <c r="D162" s="16">
         <v>0</v>
       </c>
-      <c r="E162" s="16" t="s">
+      <c r="E162" s="15" t="s">
         <v>65</v>
       </c>
     </row>
@@ -8192,10 +8192,10 @@
       <c r="C163">
         <v>2016</v>
       </c>
-      <c r="D163" s="15">
+      <c r="D163" s="16">
         <v>0</v>
       </c>
-      <c r="E163" s="16" t="s">
+      <c r="E163" s="15" t="s">
         <v>65</v>
       </c>
     </row>
@@ -8209,10 +8209,10 @@
       <c r="C164">
         <v>2016</v>
       </c>
-      <c r="D164" s="15">
+      <c r="D164" s="16">
         <v>0</v>
       </c>
-      <c r="E164" s="16" t="s">
+      <c r="E164" s="15" t="s">
         <v>65</v>
       </c>
     </row>
@@ -8226,10 +8226,10 @@
       <c r="C165">
         <v>2016</v>
       </c>
-      <c r="D165" s="15">
+      <c r="D165" s="16">
         <v>0</v>
       </c>
-      <c r="E165" s="16" t="s">
+      <c r="E165" s="15" t="s">
         <v>65</v>
       </c>
     </row>
@@ -8243,10 +8243,10 @@
       <c r="C166">
         <v>2016</v>
       </c>
-      <c r="D166" s="15">
+      <c r="D166" s="16">
         <v>0</v>
       </c>
-      <c r="E166" s="16" t="s">
+      <c r="E166" s="15" t="s">
         <v>65</v>
       </c>
     </row>
@@ -8260,10 +8260,10 @@
       <c r="C167">
         <v>2016</v>
       </c>
-      <c r="D167" s="15">
+      <c r="D167" s="16">
         <v>0</v>
       </c>
-      <c r="E167" s="16" t="s">
+      <c r="E167" s="15" t="s">
         <v>65</v>
       </c>
     </row>
@@ -8277,10 +8277,10 @@
       <c r="C168">
         <v>2016</v>
       </c>
-      <c r="D168" s="15">
+      <c r="D168" s="16">
         <v>0</v>
       </c>
-      <c r="E168" s="16" t="s">
+      <c r="E168" s="15" t="s">
         <v>65</v>
       </c>
     </row>
@@ -8294,10 +8294,10 @@
       <c r="C169">
         <v>2016</v>
       </c>
-      <c r="D169" s="15">
+      <c r="D169" s="16">
         <v>0</v>
       </c>
-      <c r="E169" s="16" t="s">
+      <c r="E169" s="15" t="s">
         <v>65</v>
       </c>
     </row>
@@ -8311,10 +8311,10 @@
       <c r="C170">
         <v>2016</v>
       </c>
-      <c r="D170" s="15">
+      <c r="D170" s="16">
         <v>0</v>
       </c>
-      <c r="E170" s="16" t="s">
+      <c r="E170" s="15" t="s">
         <v>65</v>
       </c>
     </row>
@@ -8328,10 +8328,10 @@
       <c r="C171">
         <v>2016</v>
       </c>
-      <c r="D171" s="15">
+      <c r="D171" s="16">
         <v>0</v>
       </c>
-      <c r="E171" s="16" t="s">
+      <c r="E171" s="15" t="s">
         <v>65</v>
       </c>
     </row>
@@ -8345,10 +8345,10 @@
       <c r="C172">
         <v>2016</v>
       </c>
-      <c r="D172" s="15">
+      <c r="D172" s="16">
         <v>0</v>
       </c>
-      <c r="E172" s="16" t="s">
+      <c r="E172" s="15" t="s">
         <v>65</v>
       </c>
     </row>
@@ -8362,10 +8362,10 @@
       <c r="C173">
         <v>2016</v>
       </c>
-      <c r="D173" s="15">
+      <c r="D173" s="16">
         <v>0</v>
       </c>
-      <c r="E173" s="16" t="s">
+      <c r="E173" s="15" t="s">
         <v>65</v>
       </c>
     </row>
@@ -8379,10 +8379,10 @@
       <c r="C174">
         <v>2016</v>
       </c>
-      <c r="D174" s="15">
+      <c r="D174" s="16">
         <v>0</v>
       </c>
-      <c r="E174" s="16" t="s">
+      <c r="E174" s="15" t="s">
         <v>65</v>
       </c>
     </row>
@@ -8396,10 +8396,10 @@
       <c r="C175">
         <v>2016</v>
       </c>
-      <c r="D175" s="15">
+      <c r="D175" s="16">
         <v>0</v>
       </c>
-      <c r="E175" s="16" t="s">
+      <c r="E175" s="15" t="s">
         <v>65</v>
       </c>
     </row>
@@ -8413,10 +8413,10 @@
       <c r="C176">
         <v>2016</v>
       </c>
-      <c r="D176" s="15">
+      <c r="D176" s="16">
         <v>0</v>
       </c>
-      <c r="E176" s="16" t="s">
+      <c r="E176" s="15" t="s">
         <v>65</v>
       </c>
     </row>
@@ -8430,10 +8430,10 @@
       <c r="C177">
         <v>2016</v>
       </c>
-      <c r="D177" s="15">
+      <c r="D177" s="16">
         <v>0</v>
       </c>
-      <c r="E177" s="16" t="s">
+      <c r="E177" s="15" t="s">
         <v>65</v>
       </c>
     </row>
@@ -8447,10 +8447,10 @@
       <c r="C178">
         <v>2016</v>
       </c>
-      <c r="D178" s="15">
+      <c r="D178" s="16">
         <v>0</v>
       </c>
-      <c r="E178" s="16" t="s">
+      <c r="E178" s="15" t="s">
         <v>65</v>
       </c>
     </row>
@@ -8464,10 +8464,10 @@
       <c r="C179">
         <v>2016</v>
       </c>
-      <c r="D179" s="15">
+      <c r="D179" s="16">
         <v>0</v>
       </c>
-      <c r="E179" s="16" t="s">
+      <c r="E179" s="15" t="s">
         <v>65</v>
       </c>
     </row>
@@ -8481,10 +8481,10 @@
       <c r="C180">
         <v>2016</v>
       </c>
-      <c r="D180" s="15">
+      <c r="D180" s="16">
         <v>0</v>
       </c>
-      <c r="E180" s="16" t="s">
+      <c r="E180" s="15" t="s">
         <v>65</v>
       </c>
     </row>
@@ -8498,10 +8498,10 @@
       <c r="C181">
         <v>2016</v>
       </c>
-      <c r="D181" s="15">
+      <c r="D181" s="16">
         <v>0</v>
       </c>
-      <c r="E181" s="16" t="s">
+      <c r="E181" s="15" t="s">
         <v>65</v>
       </c>
     </row>
@@ -8515,10 +8515,10 @@
       <c r="C182">
         <v>2016</v>
       </c>
-      <c r="D182" s="15">
+      <c r="D182" s="16">
         <v>0</v>
       </c>
-      <c r="E182" s="16" t="s">
+      <c r="E182" s="15" t="s">
         <v>65</v>
       </c>
     </row>
@@ -8532,10 +8532,10 @@
       <c r="C183">
         <v>2016</v>
       </c>
-      <c r="D183" s="15">
+      <c r="D183" s="16">
         <v>0</v>
       </c>
-      <c r="E183" s="16" t="s">
+      <c r="E183" s="15" t="s">
         <v>65</v>
       </c>
     </row>
@@ -8549,10 +8549,10 @@
       <c r="C184">
         <v>2016</v>
       </c>
-      <c r="D184" s="15">
+      <c r="D184" s="16">
         <v>0</v>
       </c>
-      <c r="E184" s="16" t="s">
+      <c r="E184" s="15" t="s">
         <v>65</v>
       </c>
     </row>
@@ -8566,10 +8566,10 @@
       <c r="C185">
         <v>2016</v>
       </c>
-      <c r="D185" s="15">
+      <c r="D185" s="16">
         <v>0</v>
       </c>
-      <c r="E185" s="16" t="s">
+      <c r="E185" s="15" t="s">
         <v>65</v>
       </c>
     </row>
@@ -8583,10 +8583,10 @@
       <c r="C186">
         <v>2016</v>
       </c>
-      <c r="D186" s="15">
+      <c r="D186" s="16">
         <v>0</v>
       </c>
-      <c r="E186" s="16" t="s">
+      <c r="E186" s="15" t="s">
         <v>65</v>
       </c>
     </row>
@@ -8600,10 +8600,10 @@
       <c r="C187">
         <v>2016</v>
       </c>
-      <c r="D187" s="15">
+      <c r="D187" s="16">
         <v>0</v>
       </c>
-      <c r="E187" s="16" t="s">
+      <c r="E187" s="15" t="s">
         <v>65</v>
       </c>
     </row>

</xml_diff>